<commit_message>
Update Code to website
Include website for missing packages.
</commit_message>
<xml_diff>
--- a/data_script/Rpackages/packages_status.xlsx
+++ b/data_script/Rpackages/packages_status.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+  <si>
+    <t xml:space="preserve">Workbook created using Rpackage_status.R. Code needs to be rerun with each new install.</t>
+  </si>
   <si>
     <t xml:space="preserve">Requires IT (Mike) to install</t>
   </si>
@@ -26,6 +29,9 @@
     <t xml:space="preserve">Missing Package notes</t>
   </si>
   <si>
+    <t xml:space="preserve">Missing Package Download Site</t>
+  </si>
+  <si>
     <t xml:space="preserve">abc</t>
   </si>
   <si>
@@ -602,46 +608,70 @@
     <t xml:space="preserve">contains an .exe file, permission denied</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/processx/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">callr</t>
   </si>
   <si>
     <t xml:space="preserve">requires processx</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/callr/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">reprex</t>
   </si>
   <si>
     <t xml:space="preserve">requires processx and callr</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/reprex/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">rvest</t>
   </si>
   <si>
     <t xml:space="preserve">unable to overwrite previous install</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/rvest/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">tidyverse</t>
   </si>
   <si>
     <t xml:space="preserve">requires all packages listed above</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/tidyverse/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">rgdal</t>
   </si>
   <si>
     <t xml:space="preserve">contains .MID file, permission denied</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/rgdal/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">tigris</t>
   </si>
   <si>
     <t xml:space="preserve">requires rgdal</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/tigris/index.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">choroplethr</t>
   </si>
   <si>
     <t xml:space="preserve">requires rgdal and tigris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cran.r-project.org/web/packages/choroplethr/index.html</t>
   </si>
 </sst>
 </file>
@@ -1001,1020 +1031,1053 @@
     <col min="1" max="1" width="27.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="27.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="40.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="71.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>195</v>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>197</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>203</v>
+      </c>
+      <c r="D7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>206</v>
+      </c>
+      <c r="D8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>205</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" t="s">
-        <v>207</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>209</v>
+        <v>215</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>